<commit_message>
Major Updates - Scenario, etc.
</commit_message>
<xml_diff>
--- a/TECHNIC/support/mev_type.xlsx
+++ b/TECHNIC/support/mev_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9899d96411bbb4a3/Git/Project_LEGO/TECHNIC/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_F25DC773A252ABDACC1048B1B99E47D05ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15A4A3D7-4E82-4AB3-A3C9-3D3042D5E224}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_F25DC773A252ABDACC1048B1B99E47D05ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{982F7219-9759-4AF7-B889-03082FE211BE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>mev_code</t>
   </si>
@@ -36,9 +36,6 @@
     <t>level</t>
   </si>
   <si>
-    <t>M1</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -49,6 +46,36 @@
   </si>
   <si>
     <t>CPI</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Nominal GDP</t>
+  </si>
+  <si>
+    <t>Personal Savings Rate</t>
+  </si>
+  <si>
+    <t>Personal Disposable Income</t>
+  </si>
+  <si>
+    <t>Unemployment Rate</t>
+  </si>
+  <si>
+    <t>Consumer Price Index</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>PSR</t>
+  </si>
+  <si>
+    <t>UNRATE</t>
   </si>
 </sst>
 </file>
@@ -101,6 +128,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,58 +397,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>